<commit_message>
perbaikan & penambahan data mahasiswa
</commit_message>
<xml_diff>
--- a/S1 Keperawatan/RPL/RPL 1/Transkip RPL 1.xlsx
+++ b/S1 Keperawatan/RPL/RPL 1/Transkip RPL 1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nando\Documents\Stikes\transkip_nilai_2025\S1 Keperawatan\RPL\RPL 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nando\Documents\Stikes\Transkip Nilai 2025\S1 Keperawatan\RPL\RPL 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D2D8BB-BC75-46DE-94E0-A494B1FD8CE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E53407E-0069-43DB-8783-03A9735619F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C623B17B-F356-4211-B3E1-9052FF0B64E1}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="101">
   <si>
     <t>NO</t>
   </si>
@@ -334,6 +334,9 @@
   </si>
   <si>
     <t>06 Oktober 2025</t>
+  </si>
+  <si>
+    <t>Pengaruh Pemberian Terapi Musik Terhadap Kecemasan Pasien Anak Toodler Usia 1-3 Tahun Pada Pemasangan Infus Di Ruang Lotus Rsbk Batam</t>
   </si>
 </sst>
 </file>
@@ -499,23 +502,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -526,7 +518,18 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -845,7 +848,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" topLeftCell="EK1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G21" sqref="G21"/>
+      <selection pane="topRight" activeCell="FC7" sqref="FC7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1005,262 +1008,262 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:159" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="26" t="s">
+      <c r="C1" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24" t="s">
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="24"/>
-      <c r="O1" s="24"/>
-      <c r="P1" s="24"/>
-      <c r="Q1" s="24"/>
-      <c r="R1" s="24" t="s">
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="20"/>
+      <c r="Q1" s="20"/>
+      <c r="R1" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="S1" s="24"/>
-      <c r="T1" s="24"/>
-      <c r="U1" s="24"/>
-      <c r="V1" s="24"/>
-      <c r="W1" s="24" t="s">
+      <c r="S1" s="20"/>
+      <c r="T1" s="20"/>
+      <c r="U1" s="20"/>
+      <c r="V1" s="20"/>
+      <c r="W1" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="X1" s="24"/>
-      <c r="Y1" s="24"/>
-      <c r="Z1" s="24"/>
-      <c r="AA1" s="24"/>
-      <c r="AB1" s="24" t="s">
+      <c r="X1" s="20"/>
+      <c r="Y1" s="20"/>
+      <c r="Z1" s="20"/>
+      <c r="AA1" s="20"/>
+      <c r="AB1" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="AC1" s="24"/>
-      <c r="AD1" s="24"/>
-      <c r="AE1" s="24"/>
-      <c r="AF1" s="24"/>
-      <c r="AG1" s="24" t="s">
+      <c r="AC1" s="20"/>
+      <c r="AD1" s="20"/>
+      <c r="AE1" s="20"/>
+      <c r="AF1" s="20"/>
+      <c r="AG1" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="AH1" s="24"/>
-      <c r="AI1" s="24"/>
-      <c r="AJ1" s="24"/>
-      <c r="AK1" s="24"/>
-      <c r="AL1" s="24" t="s">
+      <c r="AH1" s="20"/>
+      <c r="AI1" s="20"/>
+      <c r="AJ1" s="20"/>
+      <c r="AK1" s="20"/>
+      <c r="AL1" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="AM1" s="24"/>
-      <c r="AN1" s="24"/>
-      <c r="AO1" s="24"/>
-      <c r="AP1" s="24"/>
-      <c r="AQ1" s="24" t="s">
+      <c r="AM1" s="20"/>
+      <c r="AN1" s="20"/>
+      <c r="AO1" s="20"/>
+      <c r="AP1" s="20"/>
+      <c r="AQ1" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="AR1" s="24"/>
-      <c r="AS1" s="24"/>
-      <c r="AT1" s="24"/>
-      <c r="AU1" s="24"/>
-      <c r="AV1" s="24" t="s">
+      <c r="AR1" s="20"/>
+      <c r="AS1" s="20"/>
+      <c r="AT1" s="20"/>
+      <c r="AU1" s="20"/>
+      <c r="AV1" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="AW1" s="24"/>
-      <c r="AX1" s="24"/>
-      <c r="AY1" s="24"/>
-      <c r="AZ1" s="24"/>
-      <c r="BA1" s="23" t="s">
+      <c r="AW1" s="20"/>
+      <c r="AX1" s="20"/>
+      <c r="AY1" s="20"/>
+      <c r="AZ1" s="20"/>
+      <c r="BA1" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="BB1" s="23"/>
-      <c r="BC1" s="23"/>
-      <c r="BD1" s="23"/>
-      <c r="BE1" s="23"/>
-      <c r="BF1" s="23" t="s">
+      <c r="BB1" s="26"/>
+      <c r="BC1" s="26"/>
+      <c r="BD1" s="26"/>
+      <c r="BE1" s="26"/>
+      <c r="BF1" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="BG1" s="23"/>
-      <c r="BH1" s="23"/>
-      <c r="BI1" s="23"/>
-      <c r="BJ1" s="23"/>
-      <c r="BK1" s="23" t="s">
+      <c r="BG1" s="26"/>
+      <c r="BH1" s="26"/>
+      <c r="BI1" s="26"/>
+      <c r="BJ1" s="26"/>
+      <c r="BK1" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="BL1" s="23"/>
-      <c r="BM1" s="23"/>
-      <c r="BN1" s="23"/>
-      <c r="BO1" s="23"/>
-      <c r="BP1" s="23" t="s">
+      <c r="BL1" s="26"/>
+      <c r="BM1" s="26"/>
+      <c r="BN1" s="26"/>
+      <c r="BO1" s="26"/>
+      <c r="BP1" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="BQ1" s="23"/>
-      <c r="BR1" s="23"/>
-      <c r="BS1" s="23"/>
-      <c r="BT1" s="23"/>
-      <c r="BU1" s="23" t="s">
+      <c r="BQ1" s="26"/>
+      <c r="BR1" s="26"/>
+      <c r="BS1" s="26"/>
+      <c r="BT1" s="26"/>
+      <c r="BU1" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="BV1" s="23"/>
-      <c r="BW1" s="23"/>
-      <c r="BX1" s="23"/>
-      <c r="BY1" s="23"/>
-      <c r="BZ1" s="23" t="s">
+      <c r="BV1" s="26"/>
+      <c r="BW1" s="26"/>
+      <c r="BX1" s="26"/>
+      <c r="BY1" s="26"/>
+      <c r="BZ1" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="CA1" s="23"/>
-      <c r="CB1" s="23"/>
-      <c r="CC1" s="23"/>
-      <c r="CD1" s="23"/>
-      <c r="CE1" s="23" t="s">
+      <c r="CA1" s="26"/>
+      <c r="CB1" s="26"/>
+      <c r="CC1" s="26"/>
+      <c r="CD1" s="26"/>
+      <c r="CE1" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="CF1" s="23"/>
-      <c r="CG1" s="23"/>
-      <c r="CH1" s="23"/>
-      <c r="CI1" s="23"/>
-      <c r="CJ1" s="23" t="s">
+      <c r="CF1" s="26"/>
+      <c r="CG1" s="26"/>
+      <c r="CH1" s="26"/>
+      <c r="CI1" s="26"/>
+      <c r="CJ1" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="CK1" s="23"/>
-      <c r="CL1" s="23"/>
-      <c r="CM1" s="23"/>
-      <c r="CN1" s="23"/>
-      <c r="CO1" s="23" t="s">
+      <c r="CK1" s="26"/>
+      <c r="CL1" s="26"/>
+      <c r="CM1" s="26"/>
+      <c r="CN1" s="26"/>
+      <c r="CO1" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="CP1" s="23"/>
-      <c r="CQ1" s="23"/>
-      <c r="CR1" s="23"/>
-      <c r="CS1" s="23"/>
-      <c r="CT1" s="23" t="s">
+      <c r="CP1" s="26"/>
+      <c r="CQ1" s="26"/>
+      <c r="CR1" s="26"/>
+      <c r="CS1" s="26"/>
+      <c r="CT1" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="CU1" s="23"/>
-      <c r="CV1" s="23"/>
-      <c r="CW1" s="23"/>
-      <c r="CX1" s="23"/>
-      <c r="CY1" s="22" t="s">
+      <c r="CU1" s="26"/>
+      <c r="CV1" s="26"/>
+      <c r="CW1" s="26"/>
+      <c r="CX1" s="26"/>
+      <c r="CY1" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="CZ1" s="22"/>
-      <c r="DA1" s="22"/>
-      <c r="DB1" s="22"/>
-      <c r="DC1" s="22"/>
-      <c r="DD1" s="22" t="s">
+      <c r="CZ1" s="25"/>
+      <c r="DA1" s="25"/>
+      <c r="DB1" s="25"/>
+      <c r="DC1" s="25"/>
+      <c r="DD1" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="DE1" s="22"/>
-      <c r="DF1" s="22"/>
-      <c r="DG1" s="22"/>
-      <c r="DH1" s="22"/>
-      <c r="DI1" s="22" t="s">
+      <c r="DE1" s="25"/>
+      <c r="DF1" s="25"/>
+      <c r="DG1" s="25"/>
+      <c r="DH1" s="25"/>
+      <c r="DI1" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="DJ1" s="22"/>
-      <c r="DK1" s="22"/>
-      <c r="DL1" s="22"/>
-      <c r="DM1" s="22"/>
-      <c r="DN1" s="22" t="s">
+      <c r="DJ1" s="25"/>
+      <c r="DK1" s="25"/>
+      <c r="DL1" s="25"/>
+      <c r="DM1" s="25"/>
+      <c r="DN1" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="DO1" s="22"/>
-      <c r="DP1" s="22"/>
-      <c r="DQ1" s="22"/>
-      <c r="DR1" s="22"/>
-      <c r="DS1" s="22" t="s">
+      <c r="DO1" s="25"/>
+      <c r="DP1" s="25"/>
+      <c r="DQ1" s="25"/>
+      <c r="DR1" s="25"/>
+      <c r="DS1" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="DT1" s="22"/>
-      <c r="DU1" s="22"/>
-      <c r="DV1" s="22"/>
-      <c r="DW1" s="22"/>
-      <c r="DX1" s="22" t="s">
+      <c r="DT1" s="25"/>
+      <c r="DU1" s="25"/>
+      <c r="DV1" s="25"/>
+      <c r="DW1" s="25"/>
+      <c r="DX1" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="DY1" s="22"/>
-      <c r="DZ1" s="22"/>
-      <c r="EA1" s="22"/>
-      <c r="EB1" s="22"/>
-      <c r="EC1" s="22" t="s">
+      <c r="DY1" s="25"/>
+      <c r="DZ1" s="25"/>
+      <c r="EA1" s="25"/>
+      <c r="EB1" s="25"/>
+      <c r="EC1" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="ED1" s="22"/>
-      <c r="EE1" s="22"/>
-      <c r="EF1" s="22"/>
-      <c r="EG1" s="22"/>
-      <c r="EH1" s="22" t="s">
+      <c r="ED1" s="25"/>
+      <c r="EE1" s="25"/>
+      <c r="EF1" s="25"/>
+      <c r="EG1" s="25"/>
+      <c r="EH1" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="EI1" s="22"/>
-      <c r="EJ1" s="22"/>
-      <c r="EK1" s="22"/>
-      <c r="EL1" s="22"/>
-      <c r="EM1" s="22" t="s">
+      <c r="EI1" s="25"/>
+      <c r="EJ1" s="25"/>
+      <c r="EK1" s="25"/>
+      <c r="EL1" s="25"/>
+      <c r="EM1" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="EN1" s="22"/>
-      <c r="EO1" s="22"/>
-      <c r="EP1" s="22"/>
-      <c r="EQ1" s="22"/>
-      <c r="ER1" s="20" t="s">
+      <c r="EN1" s="25"/>
+      <c r="EO1" s="25"/>
+      <c r="EP1" s="25"/>
+      <c r="EQ1" s="25"/>
+      <c r="ER1" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="ES1" s="20"/>
-      <c r="ET1" s="20" t="s">
+      <c r="ES1" s="27"/>
+      <c r="ET1" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="EU1" s="20"/>
-      <c r="EV1" s="20" t="s">
+      <c r="EU1" s="27"/>
+      <c r="EV1" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="EW1" s="20"/>
-      <c r="EX1" s="21" t="s">
+      <c r="EW1" s="27"/>
+      <c r="EX1" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="EY1" s="21" t="s">
+      <c r="EY1" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="EZ1" s="19" t="s">
+      <c r="EZ1" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="FA1" s="19" t="s">
+      <c r="FA1" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="FB1" s="19" t="s">
+      <c r="FB1" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="FC1" s="19" t="s">
+      <c r="FC1" s="21" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:159" x14ac:dyDescent="0.2">
-      <c r="A2" s="19"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="19"/>
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="21"/>
       <c r="H2" s="4" t="s">
         <v>6</v>
       </c>
@@ -1699,18 +1702,18 @@
       <c r="EW2" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="EX2" s="21"/>
-      <c r="EY2" s="21"/>
-      <c r="EZ2" s="19"/>
-      <c r="FA2" s="19"/>
-      <c r="FB2" s="19"/>
-      <c r="FC2" s="19"/>
+      <c r="EX2" s="28"/>
+      <c r="EY2" s="28"/>
+      <c r="EZ2" s="21"/>
+      <c r="FA2" s="21"/>
+      <c r="FB2" s="21"/>
+      <c r="FC2" s="21"/>
     </row>
     <row r="3" spans="1:159" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>1</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="19" t="s">
         <v>33</v>
       </c>
       <c r="C3" s="7">
@@ -3996,7 +3999,7 @@
       <c r="A7" s="7">
         <v>5</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="19" t="s">
         <v>27</v>
       </c>
       <c r="C7" s="7">
@@ -4560,7 +4563,9 @@
         <f t="shared" si="121"/>
         <v>Excellent</v>
       </c>
-      <c r="FC7" s="6"/>
+      <c r="FC7" s="6" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="8" spans="1:159" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
@@ -5706,7 +5711,7 @@
       <c r="A10" s="7">
         <v>8</v>
       </c>
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="19" t="s">
         <v>29</v>
       </c>
       <c r="C10" s="7">
@@ -6276,7 +6281,7 @@
       <c r="A11" s="7">
         <v>9</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="19" t="s">
         <v>24</v>
       </c>
       <c r="C11" s="7">
@@ -7414,7 +7419,7 @@
       <c r="A13" s="7">
         <v>11</v>
       </c>
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="19" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="7">
@@ -7984,7 +7989,7 @@
       <c r="A14" s="7">
         <v>12</v>
       </c>
-      <c r="B14" s="28" t="s">
+      <c r="B14" s="19" t="s">
         <v>31</v>
       </c>
       <c r="C14" s="7">
@@ -8550,7 +8555,7 @@
       <c r="A15" s="7">
         <v>13</v>
       </c>
-      <c r="B15" s="28" t="s">
+      <c r="B15" s="19" t="s">
         <v>32</v>
       </c>
       <c r="C15" s="7">
@@ -9693,6 +9698,34 @@
     </row>
   </sheetData>
   <mergeCells count="44">
+    <mergeCell ref="FB1:FB2"/>
+    <mergeCell ref="FC1:FC2"/>
+    <mergeCell ref="ET1:EU1"/>
+    <mergeCell ref="EV1:EW1"/>
+    <mergeCell ref="EX1:EX2"/>
+    <mergeCell ref="EY1:EY2"/>
+    <mergeCell ref="EZ1:EZ2"/>
+    <mergeCell ref="FA1:FA2"/>
+    <mergeCell ref="EM1:EQ1"/>
+    <mergeCell ref="DI1:DM1"/>
+    <mergeCell ref="ER1:ES1"/>
+    <mergeCell ref="DN1:DR1"/>
+    <mergeCell ref="DS1:DW1"/>
+    <mergeCell ref="DX1:EB1"/>
+    <mergeCell ref="EC1:EG1"/>
+    <mergeCell ref="EH1:EL1"/>
+    <mergeCell ref="DD1:DH1"/>
+    <mergeCell ref="BA1:BE1"/>
+    <mergeCell ref="BF1:BJ1"/>
+    <mergeCell ref="BK1:BO1"/>
+    <mergeCell ref="BP1:BT1"/>
+    <mergeCell ref="BU1:BY1"/>
+    <mergeCell ref="BZ1:CD1"/>
+    <mergeCell ref="CE1:CI1"/>
+    <mergeCell ref="CJ1:CN1"/>
+    <mergeCell ref="CO1:CS1"/>
+    <mergeCell ref="CT1:CX1"/>
+    <mergeCell ref="CY1:DC1"/>
     <mergeCell ref="AQ1:AU1"/>
     <mergeCell ref="AV1:AZ1"/>
     <mergeCell ref="A1:A2"/>
@@ -9709,34 +9742,6 @@
     <mergeCell ref="AG1:AK1"/>
     <mergeCell ref="AL1:AP1"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="DD1:DH1"/>
-    <mergeCell ref="BA1:BE1"/>
-    <mergeCell ref="BF1:BJ1"/>
-    <mergeCell ref="BK1:BO1"/>
-    <mergeCell ref="BP1:BT1"/>
-    <mergeCell ref="BU1:BY1"/>
-    <mergeCell ref="BZ1:CD1"/>
-    <mergeCell ref="CE1:CI1"/>
-    <mergeCell ref="CJ1:CN1"/>
-    <mergeCell ref="CO1:CS1"/>
-    <mergeCell ref="CT1:CX1"/>
-    <mergeCell ref="CY1:DC1"/>
-    <mergeCell ref="EM1:EQ1"/>
-    <mergeCell ref="DI1:DM1"/>
-    <mergeCell ref="ER1:ES1"/>
-    <mergeCell ref="DN1:DR1"/>
-    <mergeCell ref="DS1:DW1"/>
-    <mergeCell ref="DX1:EB1"/>
-    <mergeCell ref="EC1:EG1"/>
-    <mergeCell ref="EH1:EL1"/>
-    <mergeCell ref="FB1:FB2"/>
-    <mergeCell ref="FC1:FC2"/>
-    <mergeCell ref="ET1:EU1"/>
-    <mergeCell ref="EV1:EW1"/>
-    <mergeCell ref="EX1:EX2"/>
-    <mergeCell ref="EY1:EY2"/>
-    <mergeCell ref="EZ1:EZ2"/>
-    <mergeCell ref="FA1:FA2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
penambahan data mahasiswa RPL
</commit_message>
<xml_diff>
--- a/S1 Keperawatan/RPL/RPL 1/Transkip RPL 1.xlsx
+++ b/S1 Keperawatan/RPL/RPL 1/Transkip RPL 1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nando\Documents\Stikes\Transkip Nilai 2025\S1 Keperawatan\RPL\RPL 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E53407E-0069-43DB-8783-03A9735619F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BBDE79D-F968-41EA-95CE-D83F6A56169A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C623B17B-F356-4211-B3E1-9052FF0B64E1}"/>
+    <workbookView xWindow="-21697" yWindow="-2460" windowWidth="21795" windowHeight="12975" xr2:uid="{C623B17B-F356-4211-B3E1-9052FF0B64E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Transkip" sheetId="1" r:id="rId1"/>
@@ -96,9 +96,6 @@
     <t>Keselamatan Pasien Dan Keselamatan Kesehatan Kerja Dalam Keperawatan</t>
   </si>
   <si>
-    <t>Dian Sukma Dewi</t>
-  </si>
-  <si>
     <t>Putri Denanda Tami</t>
   </si>
   <si>
@@ -337,6 +334,9 @@
   </si>
   <si>
     <t>Pengaruh Pemberian Terapi Musik Terhadap Kecemasan Pasien Anak Toodler Usia 1-3 Tahun Pada Pemasangan Infus Di Ruang Lotus Rsbk Batam</t>
+  </si>
+  <si>
+    <t>Dian Sukmadewi</t>
   </si>
 </sst>
 </file>
@@ -503,11 +503,23 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -517,18 +529,6 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -847,423 +847,423 @@
   <dimension ref="A1:FC17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="EK1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="FC7" sqref="FC7"/>
+      <pane xSplit="3" topLeftCell="CK1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="CW19" sqref="CW19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="6.86328125" style="2" customWidth="1"/>
     <col min="2" max="2" width="35" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" style="1" customWidth="1"/>
-    <col min="5" max="6" width="18.28515625" style="16" customWidth="1"/>
+    <col min="3" max="3" width="18.3984375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="22.265625" style="1" customWidth="1"/>
+    <col min="5" max="6" width="18.265625" style="16" customWidth="1"/>
     <col min="7" max="7" width="22" style="1" customWidth="1"/>
-    <col min="8" max="8" width="7.42578125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="8.5703125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="8.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="7.3984375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="8.59765625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="8.1328125" style="1" customWidth="1"/>
     <col min="11" max="11" width="8" style="1" customWidth="1"/>
-    <col min="12" max="12" width="8.5703125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="6.7109375" style="1" customWidth="1"/>
-    <col min="14" max="14" width="6.5703125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="7.140625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="6.140625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="7.7109375" style="1" customWidth="1"/>
-    <col min="18" max="18" width="7.42578125" style="1" customWidth="1"/>
-    <col min="19" max="19" width="6.5703125" style="1" customWidth="1"/>
-    <col min="20" max="20" width="7.140625" style="1" customWidth="1"/>
-    <col min="21" max="21" width="6.140625" style="1" customWidth="1"/>
-    <col min="22" max="22" width="7.7109375" style="1" customWidth="1"/>
-    <col min="23" max="23" width="6.7109375" style="1" customWidth="1"/>
-    <col min="24" max="24" width="6.5703125" style="1" customWidth="1"/>
-    <col min="25" max="25" width="7.140625" style="1" customWidth="1"/>
-    <col min="26" max="26" width="6.140625" style="1" customWidth="1"/>
-    <col min="27" max="27" width="7.7109375" style="1" customWidth="1"/>
-    <col min="28" max="28" width="6.7109375" style="1" customWidth="1"/>
-    <col min="29" max="29" width="6.5703125" style="1" customWidth="1"/>
-    <col min="30" max="30" width="7.140625" style="1" customWidth="1"/>
-    <col min="31" max="31" width="6.140625" style="1" customWidth="1"/>
-    <col min="32" max="32" width="7.7109375" style="1" customWidth="1"/>
-    <col min="33" max="33" width="6.7109375" style="1" customWidth="1"/>
-    <col min="34" max="34" width="6.5703125" style="1" customWidth="1"/>
-    <col min="35" max="35" width="7.140625" style="1" customWidth="1"/>
-    <col min="36" max="36" width="6.140625" style="1" customWidth="1"/>
-    <col min="37" max="37" width="7.7109375" style="1" customWidth="1"/>
-    <col min="38" max="38" width="6.7109375" style="1" customWidth="1"/>
-    <col min="39" max="39" width="6.5703125" style="1" customWidth="1"/>
-    <col min="40" max="40" width="7.140625" style="1" customWidth="1"/>
-    <col min="41" max="41" width="6.140625" style="1" customWidth="1"/>
-    <col min="42" max="42" width="7.7109375" style="1" customWidth="1"/>
-    <col min="43" max="43" width="6.7109375" style="1" customWidth="1"/>
-    <col min="44" max="44" width="6.5703125" style="1" customWidth="1"/>
-    <col min="45" max="45" width="7.140625" style="1" customWidth="1"/>
-    <col min="46" max="46" width="6.140625" style="1" customWidth="1"/>
-    <col min="47" max="47" width="7.7109375" style="1" customWidth="1"/>
-    <col min="48" max="48" width="6.7109375" style="1" customWidth="1"/>
-    <col min="49" max="49" width="6.5703125" style="1" customWidth="1"/>
-    <col min="50" max="50" width="7.140625" style="1" customWidth="1"/>
-    <col min="51" max="51" width="6.140625" style="1" customWidth="1"/>
-    <col min="52" max="52" width="7.7109375" style="1" customWidth="1"/>
-    <col min="53" max="53" width="6.7109375" style="2" customWidth="1"/>
-    <col min="54" max="54" width="6.5703125" style="1" customWidth="1"/>
-    <col min="55" max="55" width="7.140625" style="1" customWidth="1"/>
-    <col min="56" max="56" width="6.140625" style="1" customWidth="1"/>
-    <col min="57" max="57" width="7.7109375" style="1" customWidth="1"/>
-    <col min="58" max="58" width="6.7109375" style="1" customWidth="1"/>
-    <col min="59" max="59" width="6.5703125" style="1" customWidth="1"/>
-    <col min="60" max="60" width="7.140625" style="1" customWidth="1"/>
-    <col min="61" max="61" width="6.140625" style="1" customWidth="1"/>
-    <col min="62" max="62" width="7.7109375" style="1" customWidth="1"/>
-    <col min="63" max="63" width="6.7109375" style="1" customWidth="1"/>
-    <col min="64" max="64" width="6.5703125" style="1" customWidth="1"/>
-    <col min="65" max="65" width="7.140625" style="1" customWidth="1"/>
-    <col min="66" max="66" width="6.140625" style="1" customWidth="1"/>
-    <col min="67" max="67" width="7.7109375" style="1" customWidth="1"/>
-    <col min="68" max="68" width="6.7109375" style="1" customWidth="1"/>
-    <col min="69" max="69" width="6.5703125" style="1" customWidth="1"/>
-    <col min="70" max="70" width="7.140625" style="1" customWidth="1"/>
-    <col min="71" max="71" width="6.140625" style="1" customWidth="1"/>
-    <col min="72" max="72" width="7.7109375" style="1" customWidth="1"/>
-    <col min="73" max="73" width="6.7109375" style="1" customWidth="1"/>
-    <col min="74" max="74" width="6.5703125" style="1" customWidth="1"/>
-    <col min="75" max="75" width="7.140625" style="1" customWidth="1"/>
-    <col min="76" max="76" width="6.140625" style="1" customWidth="1"/>
-    <col min="77" max="77" width="7.7109375" style="1" customWidth="1"/>
-    <col min="78" max="78" width="6.7109375" style="1" customWidth="1"/>
-    <col min="79" max="79" width="6.5703125" style="1" customWidth="1"/>
-    <col min="80" max="80" width="7.140625" style="1" customWidth="1"/>
-    <col min="81" max="81" width="6.140625" style="1" customWidth="1"/>
-    <col min="82" max="82" width="7.7109375" style="1" customWidth="1"/>
-    <col min="83" max="83" width="6.7109375" style="1" customWidth="1"/>
-    <col min="84" max="84" width="6.5703125" style="1" customWidth="1"/>
-    <col min="85" max="85" width="7.140625" style="1" customWidth="1"/>
-    <col min="86" max="86" width="6.140625" style="1" customWidth="1"/>
-    <col min="87" max="87" width="7.7109375" style="1" customWidth="1"/>
-    <col min="88" max="88" width="6.7109375" style="1" customWidth="1"/>
-    <col min="89" max="89" width="6.5703125" style="1" customWidth="1"/>
-    <col min="90" max="90" width="7.140625" style="1" customWidth="1"/>
-    <col min="91" max="91" width="6.140625" style="1" customWidth="1"/>
-    <col min="92" max="92" width="7.7109375" style="1" customWidth="1"/>
-    <col min="93" max="93" width="6.7109375" style="1" customWidth="1"/>
-    <col min="94" max="94" width="6.5703125" style="1" customWidth="1"/>
-    <col min="95" max="95" width="7.140625" style="1" customWidth="1"/>
-    <col min="96" max="96" width="6.140625" style="1" customWidth="1"/>
-    <col min="97" max="97" width="7.7109375" style="1" customWidth="1"/>
-    <col min="98" max="98" width="6.7109375" style="1" customWidth="1"/>
-    <col min="99" max="99" width="6.5703125" style="1" customWidth="1"/>
-    <col min="100" max="100" width="7.140625" style="1" customWidth="1"/>
-    <col min="101" max="101" width="6.140625" style="1" customWidth="1"/>
-    <col min="102" max="102" width="7.7109375" style="1" customWidth="1"/>
-    <col min="103" max="103" width="6.7109375" style="1" customWidth="1"/>
-    <col min="104" max="104" width="6.5703125" style="1" customWidth="1"/>
-    <col min="105" max="105" width="7.140625" style="1" customWidth="1"/>
-    <col min="106" max="106" width="6.140625" style="1" customWidth="1"/>
-    <col min="107" max="107" width="7.7109375" style="1" customWidth="1"/>
-    <col min="108" max="108" width="6.7109375" style="1" customWidth="1"/>
-    <col min="109" max="109" width="6.5703125" style="1" customWidth="1"/>
-    <col min="110" max="110" width="7.140625" style="1" customWidth="1"/>
-    <col min="111" max="111" width="6.140625" style="1" customWidth="1"/>
-    <col min="112" max="112" width="7.7109375" style="1" customWidth="1"/>
-    <col min="113" max="113" width="6.7109375" style="1" customWidth="1"/>
-    <col min="114" max="114" width="6.5703125" style="1" customWidth="1"/>
-    <col min="115" max="115" width="7.140625" style="1" customWidth="1"/>
-    <col min="116" max="116" width="6.140625" style="1" customWidth="1"/>
-    <col min="117" max="117" width="7.7109375" style="1" customWidth="1"/>
-    <col min="118" max="118" width="6.7109375" style="1" customWidth="1"/>
-    <col min="119" max="119" width="6.5703125" style="1" customWidth="1"/>
-    <col min="120" max="120" width="7.140625" style="1" customWidth="1"/>
-    <col min="121" max="121" width="6.140625" style="1" customWidth="1"/>
-    <col min="122" max="122" width="7.7109375" style="1" customWidth="1"/>
-    <col min="123" max="123" width="6.7109375" style="1" customWidth="1"/>
-    <col min="124" max="124" width="6.5703125" style="1" customWidth="1"/>
-    <col min="125" max="125" width="7.140625" style="1" customWidth="1"/>
-    <col min="126" max="126" width="6.140625" style="1" customWidth="1"/>
-    <col min="127" max="127" width="7.7109375" style="1" customWidth="1"/>
-    <col min="128" max="128" width="6.7109375" style="1" customWidth="1"/>
-    <col min="129" max="129" width="6.5703125" style="1" customWidth="1"/>
-    <col min="130" max="130" width="7.140625" style="1" customWidth="1"/>
-    <col min="131" max="131" width="6.140625" style="1" customWidth="1"/>
-    <col min="132" max="132" width="7.7109375" style="1" customWidth="1"/>
-    <col min="133" max="133" width="6.7109375" style="1" customWidth="1"/>
-    <col min="134" max="134" width="6.5703125" style="1" customWidth="1"/>
-    <col min="135" max="135" width="7.140625" style="1" customWidth="1"/>
-    <col min="136" max="136" width="6.140625" style="1" customWidth="1"/>
-    <col min="137" max="137" width="7.7109375" style="1" customWidth="1"/>
-    <col min="138" max="138" width="6.7109375" style="1" customWidth="1"/>
-    <col min="139" max="139" width="6.5703125" style="1" customWidth="1"/>
-    <col min="140" max="140" width="7.140625" style="1" customWidth="1"/>
-    <col min="141" max="141" width="6.140625" style="1" customWidth="1"/>
-    <col min="142" max="142" width="7.7109375" style="1" customWidth="1"/>
-    <col min="143" max="143" width="6.7109375" style="1" customWidth="1"/>
-    <col min="144" max="144" width="6.5703125" style="1" customWidth="1"/>
-    <col min="145" max="145" width="7.140625" style="1" customWidth="1"/>
-    <col min="146" max="146" width="6.140625" style="1" customWidth="1"/>
-    <col min="147" max="147" width="7.7109375" style="1" customWidth="1"/>
-    <col min="148" max="155" width="9.140625" style="1"/>
-    <col min="156" max="156" width="20.7109375" style="2" customWidth="1"/>
+    <col min="12" max="12" width="8.59765625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="6.73046875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="6.59765625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="7.1328125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="6.1328125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="7.73046875" style="1" customWidth="1"/>
+    <col min="18" max="18" width="7.3984375" style="1" customWidth="1"/>
+    <col min="19" max="19" width="6.59765625" style="1" customWidth="1"/>
+    <col min="20" max="20" width="7.1328125" style="1" customWidth="1"/>
+    <col min="21" max="21" width="6.1328125" style="1" customWidth="1"/>
+    <col min="22" max="22" width="7.73046875" style="1" customWidth="1"/>
+    <col min="23" max="23" width="6.73046875" style="1" customWidth="1"/>
+    <col min="24" max="24" width="6.59765625" style="1" customWidth="1"/>
+    <col min="25" max="25" width="7.1328125" style="1" customWidth="1"/>
+    <col min="26" max="26" width="6.1328125" style="1" customWidth="1"/>
+    <col min="27" max="27" width="7.73046875" style="1" customWidth="1"/>
+    <col min="28" max="28" width="6.73046875" style="1" customWidth="1"/>
+    <col min="29" max="29" width="6.59765625" style="1" customWidth="1"/>
+    <col min="30" max="30" width="7.1328125" style="1" customWidth="1"/>
+    <col min="31" max="31" width="6.1328125" style="1" customWidth="1"/>
+    <col min="32" max="32" width="7.73046875" style="1" customWidth="1"/>
+    <col min="33" max="33" width="6.73046875" style="1" customWidth="1"/>
+    <col min="34" max="34" width="6.59765625" style="1" customWidth="1"/>
+    <col min="35" max="35" width="7.1328125" style="1" customWidth="1"/>
+    <col min="36" max="36" width="6.1328125" style="1" customWidth="1"/>
+    <col min="37" max="37" width="7.73046875" style="1" customWidth="1"/>
+    <col min="38" max="38" width="6.73046875" style="1" customWidth="1"/>
+    <col min="39" max="39" width="6.59765625" style="1" customWidth="1"/>
+    <col min="40" max="40" width="7.1328125" style="1" customWidth="1"/>
+    <col min="41" max="41" width="6.1328125" style="1" customWidth="1"/>
+    <col min="42" max="42" width="7.73046875" style="1" customWidth="1"/>
+    <col min="43" max="43" width="6.73046875" style="1" customWidth="1"/>
+    <col min="44" max="44" width="6.59765625" style="1" customWidth="1"/>
+    <col min="45" max="45" width="7.1328125" style="1" customWidth="1"/>
+    <col min="46" max="46" width="6.1328125" style="1" customWidth="1"/>
+    <col min="47" max="47" width="7.73046875" style="1" customWidth="1"/>
+    <col min="48" max="48" width="6.73046875" style="1" customWidth="1"/>
+    <col min="49" max="49" width="6.59765625" style="1" customWidth="1"/>
+    <col min="50" max="50" width="7.1328125" style="1" customWidth="1"/>
+    <col min="51" max="51" width="6.1328125" style="1" customWidth="1"/>
+    <col min="52" max="52" width="7.73046875" style="1" customWidth="1"/>
+    <col min="53" max="53" width="6.73046875" style="2" customWidth="1"/>
+    <col min="54" max="54" width="6.59765625" style="1" customWidth="1"/>
+    <col min="55" max="55" width="7.1328125" style="1" customWidth="1"/>
+    <col min="56" max="56" width="6.1328125" style="1" customWidth="1"/>
+    <col min="57" max="57" width="7.73046875" style="1" customWidth="1"/>
+    <col min="58" max="58" width="6.73046875" style="1" customWidth="1"/>
+    <col min="59" max="59" width="6.59765625" style="1" customWidth="1"/>
+    <col min="60" max="60" width="7.1328125" style="1" customWidth="1"/>
+    <col min="61" max="61" width="6.1328125" style="1" customWidth="1"/>
+    <col min="62" max="62" width="7.73046875" style="1" customWidth="1"/>
+    <col min="63" max="63" width="6.73046875" style="1" customWidth="1"/>
+    <col min="64" max="64" width="6.59765625" style="1" customWidth="1"/>
+    <col min="65" max="65" width="7.1328125" style="1" customWidth="1"/>
+    <col min="66" max="66" width="6.1328125" style="1" customWidth="1"/>
+    <col min="67" max="67" width="7.73046875" style="1" customWidth="1"/>
+    <col min="68" max="68" width="6.73046875" style="1" customWidth="1"/>
+    <col min="69" max="69" width="6.59765625" style="1" customWidth="1"/>
+    <col min="70" max="70" width="7.1328125" style="1" customWidth="1"/>
+    <col min="71" max="71" width="6.1328125" style="1" customWidth="1"/>
+    <col min="72" max="72" width="7.73046875" style="1" customWidth="1"/>
+    <col min="73" max="73" width="6.73046875" style="1" customWidth="1"/>
+    <col min="74" max="74" width="6.59765625" style="1" customWidth="1"/>
+    <col min="75" max="75" width="7.1328125" style="1" customWidth="1"/>
+    <col min="76" max="76" width="6.1328125" style="1" customWidth="1"/>
+    <col min="77" max="77" width="7.73046875" style="1" customWidth="1"/>
+    <col min="78" max="78" width="6.73046875" style="1" customWidth="1"/>
+    <col min="79" max="79" width="6.59765625" style="1" customWidth="1"/>
+    <col min="80" max="80" width="7.1328125" style="1" customWidth="1"/>
+    <col min="81" max="81" width="6.1328125" style="1" customWidth="1"/>
+    <col min="82" max="82" width="7.73046875" style="1" customWidth="1"/>
+    <col min="83" max="83" width="6.73046875" style="1" customWidth="1"/>
+    <col min="84" max="84" width="6.59765625" style="1" customWidth="1"/>
+    <col min="85" max="85" width="7.1328125" style="1" customWidth="1"/>
+    <col min="86" max="86" width="6.1328125" style="1" customWidth="1"/>
+    <col min="87" max="87" width="7.73046875" style="1" customWidth="1"/>
+    <col min="88" max="88" width="6.73046875" style="1" customWidth="1"/>
+    <col min="89" max="89" width="6.59765625" style="1" customWidth="1"/>
+    <col min="90" max="90" width="7.1328125" style="1" customWidth="1"/>
+    <col min="91" max="91" width="6.1328125" style="1" customWidth="1"/>
+    <col min="92" max="92" width="7.73046875" style="1" customWidth="1"/>
+    <col min="93" max="93" width="6.73046875" style="1" customWidth="1"/>
+    <col min="94" max="94" width="6.59765625" style="1" customWidth="1"/>
+    <col min="95" max="95" width="7.1328125" style="1" customWidth="1"/>
+    <col min="96" max="96" width="6.1328125" style="1" customWidth="1"/>
+    <col min="97" max="97" width="7.73046875" style="1" customWidth="1"/>
+    <col min="98" max="98" width="6.73046875" style="1" customWidth="1"/>
+    <col min="99" max="99" width="6.59765625" style="1" customWidth="1"/>
+    <col min="100" max="100" width="7.1328125" style="1" customWidth="1"/>
+    <col min="101" max="101" width="6.1328125" style="1" customWidth="1"/>
+    <col min="102" max="102" width="7.73046875" style="1" customWidth="1"/>
+    <col min="103" max="103" width="6.73046875" style="1" customWidth="1"/>
+    <col min="104" max="104" width="6.59765625" style="1" customWidth="1"/>
+    <col min="105" max="105" width="7.1328125" style="1" customWidth="1"/>
+    <col min="106" max="106" width="6.1328125" style="1" customWidth="1"/>
+    <col min="107" max="107" width="7.73046875" style="1" customWidth="1"/>
+    <col min="108" max="108" width="6.73046875" style="1" customWidth="1"/>
+    <col min="109" max="109" width="6.59765625" style="1" customWidth="1"/>
+    <col min="110" max="110" width="7.1328125" style="1" customWidth="1"/>
+    <col min="111" max="111" width="6.1328125" style="1" customWidth="1"/>
+    <col min="112" max="112" width="7.73046875" style="1" customWidth="1"/>
+    <col min="113" max="113" width="6.73046875" style="1" customWidth="1"/>
+    <col min="114" max="114" width="6.59765625" style="1" customWidth="1"/>
+    <col min="115" max="115" width="7.1328125" style="1" customWidth="1"/>
+    <col min="116" max="116" width="6.1328125" style="1" customWidth="1"/>
+    <col min="117" max="117" width="7.73046875" style="1" customWidth="1"/>
+    <col min="118" max="118" width="6.73046875" style="1" customWidth="1"/>
+    <col min="119" max="119" width="6.59765625" style="1" customWidth="1"/>
+    <col min="120" max="120" width="7.1328125" style="1" customWidth="1"/>
+    <col min="121" max="121" width="6.1328125" style="1" customWidth="1"/>
+    <col min="122" max="122" width="7.73046875" style="1" customWidth="1"/>
+    <col min="123" max="123" width="6.73046875" style="1" customWidth="1"/>
+    <col min="124" max="124" width="6.59765625" style="1" customWidth="1"/>
+    <col min="125" max="125" width="7.1328125" style="1" customWidth="1"/>
+    <col min="126" max="126" width="6.1328125" style="1" customWidth="1"/>
+    <col min="127" max="127" width="7.73046875" style="1" customWidth="1"/>
+    <col min="128" max="128" width="6.73046875" style="1" customWidth="1"/>
+    <col min="129" max="129" width="6.59765625" style="1" customWidth="1"/>
+    <col min="130" max="130" width="7.1328125" style="1" customWidth="1"/>
+    <col min="131" max="131" width="6.1328125" style="1" customWidth="1"/>
+    <col min="132" max="132" width="7.73046875" style="1" customWidth="1"/>
+    <col min="133" max="133" width="6.73046875" style="1" customWidth="1"/>
+    <col min="134" max="134" width="6.59765625" style="1" customWidth="1"/>
+    <col min="135" max="135" width="7.1328125" style="1" customWidth="1"/>
+    <col min="136" max="136" width="6.1328125" style="1" customWidth="1"/>
+    <col min="137" max="137" width="7.73046875" style="1" customWidth="1"/>
+    <col min="138" max="138" width="6.73046875" style="1" customWidth="1"/>
+    <col min="139" max="139" width="6.59765625" style="1" customWidth="1"/>
+    <col min="140" max="140" width="7.1328125" style="1" customWidth="1"/>
+    <col min="141" max="141" width="6.1328125" style="1" customWidth="1"/>
+    <col min="142" max="142" width="7.73046875" style="1" customWidth="1"/>
+    <col min="143" max="143" width="6.73046875" style="1" customWidth="1"/>
+    <col min="144" max="144" width="6.59765625" style="1" customWidth="1"/>
+    <col min="145" max="145" width="7.1328125" style="1" customWidth="1"/>
+    <col min="146" max="146" width="6.1328125" style="1" customWidth="1"/>
+    <col min="147" max="147" width="7.73046875" style="1" customWidth="1"/>
+    <col min="148" max="155" width="9.1328125" style="1"/>
+    <col min="156" max="156" width="20.73046875" style="2" customWidth="1"/>
     <col min="157" max="157" width="18" style="1" customWidth="1"/>
-    <col min="158" max="158" width="18.28515625" style="1" customWidth="1"/>
-    <col min="159" max="159" width="27.7109375" style="1" customWidth="1"/>
-    <col min="160" max="16384" width="9.140625" style="1"/>
+    <col min="158" max="158" width="18.265625" style="1" customWidth="1"/>
+    <col min="159" max="159" width="27.73046875" style="1" customWidth="1"/>
+    <col min="160" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:159" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:159" x14ac:dyDescent="0.35">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="G1" s="21" t="s">
+      <c r="C1" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20" t="s">
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="20"/>
-      <c r="R1" s="20" t="s">
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="S1" s="20"/>
-      <c r="T1" s="20"/>
-      <c r="U1" s="20"/>
-      <c r="V1" s="20"/>
-      <c r="W1" s="20" t="s">
+      <c r="S1" s="25"/>
+      <c r="T1" s="25"/>
+      <c r="U1" s="25"/>
+      <c r="V1" s="25"/>
+      <c r="W1" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="X1" s="20"/>
-      <c r="Y1" s="20"/>
-      <c r="Z1" s="20"/>
-      <c r="AA1" s="20"/>
-      <c r="AB1" s="20" t="s">
+      <c r="X1" s="25"/>
+      <c r="Y1" s="25"/>
+      <c r="Z1" s="25"/>
+      <c r="AA1" s="25"/>
+      <c r="AB1" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="AC1" s="20"/>
-      <c r="AD1" s="20"/>
-      <c r="AE1" s="20"/>
-      <c r="AF1" s="20"/>
-      <c r="AG1" s="20" t="s">
+      <c r="AC1" s="25"/>
+      <c r="AD1" s="25"/>
+      <c r="AE1" s="25"/>
+      <c r="AF1" s="25"/>
+      <c r="AG1" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="AH1" s="20"/>
-      <c r="AI1" s="20"/>
-      <c r="AJ1" s="20"/>
-      <c r="AK1" s="20"/>
-      <c r="AL1" s="20" t="s">
+      <c r="AH1" s="25"/>
+      <c r="AI1" s="25"/>
+      <c r="AJ1" s="25"/>
+      <c r="AK1" s="25"/>
+      <c r="AL1" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="AM1" s="20"/>
-      <c r="AN1" s="20"/>
-      <c r="AO1" s="20"/>
-      <c r="AP1" s="20"/>
-      <c r="AQ1" s="20" t="s">
+      <c r="AM1" s="25"/>
+      <c r="AN1" s="25"/>
+      <c r="AO1" s="25"/>
+      <c r="AP1" s="25"/>
+      <c r="AQ1" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="AR1" s="20"/>
-      <c r="AS1" s="20"/>
-      <c r="AT1" s="20"/>
-      <c r="AU1" s="20"/>
-      <c r="AV1" s="20" t="s">
+      <c r="AR1" s="25"/>
+      <c r="AS1" s="25"/>
+      <c r="AT1" s="25"/>
+      <c r="AU1" s="25"/>
+      <c r="AV1" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="AW1" s="20"/>
-      <c r="AX1" s="20"/>
-      <c r="AY1" s="20"/>
-      <c r="AZ1" s="20"/>
-      <c r="BA1" s="26" t="s">
+      <c r="AW1" s="25"/>
+      <c r="AX1" s="25"/>
+      <c r="AY1" s="25"/>
+      <c r="AZ1" s="25"/>
+      <c r="BA1" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="BB1" s="24"/>
+      <c r="BC1" s="24"/>
+      <c r="BD1" s="24"/>
+      <c r="BE1" s="24"/>
+      <c r="BF1" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="BB1" s="26"/>
-      <c r="BC1" s="26"/>
-      <c r="BD1" s="26"/>
-      <c r="BE1" s="26"/>
-      <c r="BF1" s="26" t="s">
+      <c r="BG1" s="24"/>
+      <c r="BH1" s="24"/>
+      <c r="BI1" s="24"/>
+      <c r="BJ1" s="24"/>
+      <c r="BK1" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="BG1" s="26"/>
-      <c r="BH1" s="26"/>
-      <c r="BI1" s="26"/>
-      <c r="BJ1" s="26"/>
-      <c r="BK1" s="26" t="s">
+      <c r="BL1" s="24"/>
+      <c r="BM1" s="24"/>
+      <c r="BN1" s="24"/>
+      <c r="BO1" s="24"/>
+      <c r="BP1" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="BL1" s="26"/>
-      <c r="BM1" s="26"/>
-      <c r="BN1" s="26"/>
-      <c r="BO1" s="26"/>
-      <c r="BP1" s="26" t="s">
+      <c r="BQ1" s="24"/>
+      <c r="BR1" s="24"/>
+      <c r="BS1" s="24"/>
+      <c r="BT1" s="24"/>
+      <c r="BU1" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="BQ1" s="26"/>
-      <c r="BR1" s="26"/>
-      <c r="BS1" s="26"/>
-      <c r="BT1" s="26"/>
-      <c r="BU1" s="26" t="s">
+      <c r="BV1" s="24"/>
+      <c r="BW1" s="24"/>
+      <c r="BX1" s="24"/>
+      <c r="BY1" s="24"/>
+      <c r="BZ1" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="BV1" s="26"/>
-      <c r="BW1" s="26"/>
-      <c r="BX1" s="26"/>
-      <c r="BY1" s="26"/>
-      <c r="BZ1" s="26" t="s">
+      <c r="CA1" s="24"/>
+      <c r="CB1" s="24"/>
+      <c r="CC1" s="24"/>
+      <c r="CD1" s="24"/>
+      <c r="CE1" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="CA1" s="26"/>
-      <c r="CB1" s="26"/>
-      <c r="CC1" s="26"/>
-      <c r="CD1" s="26"/>
-      <c r="CE1" s="26" t="s">
+      <c r="CF1" s="24"/>
+      <c r="CG1" s="24"/>
+      <c r="CH1" s="24"/>
+      <c r="CI1" s="24"/>
+      <c r="CJ1" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="CF1" s="26"/>
-      <c r="CG1" s="26"/>
-      <c r="CH1" s="26"/>
-      <c r="CI1" s="26"/>
-      <c r="CJ1" s="26" t="s">
+      <c r="CK1" s="24"/>
+      <c r="CL1" s="24"/>
+      <c r="CM1" s="24"/>
+      <c r="CN1" s="24"/>
+      <c r="CO1" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="CK1" s="26"/>
-      <c r="CL1" s="26"/>
-      <c r="CM1" s="26"/>
-      <c r="CN1" s="26"/>
-      <c r="CO1" s="26" t="s">
+      <c r="CP1" s="24"/>
+      <c r="CQ1" s="24"/>
+      <c r="CR1" s="24"/>
+      <c r="CS1" s="24"/>
+      <c r="CT1" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="CP1" s="26"/>
-      <c r="CQ1" s="26"/>
-      <c r="CR1" s="26"/>
-      <c r="CS1" s="26"/>
-      <c r="CT1" s="26" t="s">
+      <c r="CU1" s="24"/>
+      <c r="CV1" s="24"/>
+      <c r="CW1" s="24"/>
+      <c r="CX1" s="24"/>
+      <c r="CY1" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="CU1" s="26"/>
-      <c r="CV1" s="26"/>
-      <c r="CW1" s="26"/>
-      <c r="CX1" s="26"/>
-      <c r="CY1" s="25" t="s">
+      <c r="CZ1" s="23"/>
+      <c r="DA1" s="23"/>
+      <c r="DB1" s="23"/>
+      <c r="DC1" s="23"/>
+      <c r="DD1" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="CZ1" s="25"/>
-      <c r="DA1" s="25"/>
-      <c r="DB1" s="25"/>
-      <c r="DC1" s="25"/>
-      <c r="DD1" s="25" t="s">
+      <c r="DE1" s="23"/>
+      <c r="DF1" s="23"/>
+      <c r="DG1" s="23"/>
+      <c r="DH1" s="23"/>
+      <c r="DI1" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="DJ1" s="23"/>
+      <c r="DK1" s="23"/>
+      <c r="DL1" s="23"/>
+      <c r="DM1" s="23"/>
+      <c r="DN1" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="DE1" s="25"/>
-      <c r="DF1" s="25"/>
-      <c r="DG1" s="25"/>
-      <c r="DH1" s="25"/>
-      <c r="DI1" s="25" t="s">
+      <c r="DO1" s="23"/>
+      <c r="DP1" s="23"/>
+      <c r="DQ1" s="23"/>
+      <c r="DR1" s="23"/>
+      <c r="DS1" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="DJ1" s="25"/>
-      <c r="DK1" s="25"/>
-      <c r="DL1" s="25"/>
-      <c r="DM1" s="25"/>
-      <c r="DN1" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="DO1" s="25"/>
-      <c r="DP1" s="25"/>
-      <c r="DQ1" s="25"/>
-      <c r="DR1" s="25"/>
-      <c r="DS1" s="25" t="s">
+      <c r="DT1" s="23"/>
+      <c r="DU1" s="23"/>
+      <c r="DV1" s="23"/>
+      <c r="DW1" s="23"/>
+      <c r="DX1" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="DT1" s="25"/>
-      <c r="DU1" s="25"/>
-      <c r="DV1" s="25"/>
-      <c r="DW1" s="25"/>
-      <c r="DX1" s="25" t="s">
+      <c r="DY1" s="23"/>
+      <c r="DZ1" s="23"/>
+      <c r="EA1" s="23"/>
+      <c r="EB1" s="23"/>
+      <c r="EC1" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="DY1" s="25"/>
-      <c r="DZ1" s="25"/>
-      <c r="EA1" s="25"/>
-      <c r="EB1" s="25"/>
-      <c r="EC1" s="25" t="s">
+      <c r="ED1" s="23"/>
+      <c r="EE1" s="23"/>
+      <c r="EF1" s="23"/>
+      <c r="EG1" s="23"/>
+      <c r="EH1" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="ED1" s="25"/>
-      <c r="EE1" s="25"/>
-      <c r="EF1" s="25"/>
-      <c r="EG1" s="25"/>
-      <c r="EH1" s="25" t="s">
+      <c r="EI1" s="23"/>
+      <c r="EJ1" s="23"/>
+      <c r="EK1" s="23"/>
+      <c r="EL1" s="23"/>
+      <c r="EM1" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="EI1" s="25"/>
-      <c r="EJ1" s="25"/>
-      <c r="EK1" s="25"/>
-      <c r="EL1" s="25"/>
-      <c r="EM1" s="25" t="s">
+      <c r="EN1" s="23"/>
+      <c r="EO1" s="23"/>
+      <c r="EP1" s="23"/>
+      <c r="EQ1" s="23"/>
+      <c r="ER1" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="EN1" s="25"/>
-      <c r="EO1" s="25"/>
-      <c r="EP1" s="25"/>
-      <c r="EQ1" s="25"/>
-      <c r="ER1" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="ES1" s="27"/>
-      <c r="ET1" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="EU1" s="27"/>
-      <c r="EV1" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="EW1" s="27"/>
-      <c r="EX1" s="28" t="s">
+      <c r="ES1" s="21"/>
+      <c r="ET1" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="EU1" s="21"/>
+      <c r="EV1" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="EW1" s="21"/>
+      <c r="EX1" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="EY1" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="EY1" s="28" t="s">
+      <c r="EZ1" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="EZ1" s="21" t="s">
+      <c r="FA1" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="FA1" s="21" t="s">
+      <c r="FB1" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="FB1" s="21" t="s">
+      <c r="FC1" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="FC1" s="21" t="s">
-        <v>67</v>
-      </c>
     </row>
-    <row r="2" spans="1:159" x14ac:dyDescent="0.2">
-      <c r="A2" s="21"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="21"/>
+    <row r="2" spans="1:159" x14ac:dyDescent="0.35">
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="20"/>
       <c r="H2" s="4" t="s">
         <v>6</v>
       </c>
@@ -1685,48 +1685,48 @@
         <v>10</v>
       </c>
       <c r="ER2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="ES2" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="ES2" s="6" t="s">
-        <v>55</v>
-      </c>
       <c r="ET2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="EU2" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="EU2" s="6" t="s">
-        <v>58</v>
-      </c>
       <c r="EV2" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="EW2" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="EW2" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="EX2" s="28"/>
-      <c r="EY2" s="28"/>
-      <c r="EZ2" s="21"/>
-      <c r="FA2" s="21"/>
-      <c r="FB2" s="21"/>
-      <c r="FC2" s="21"/>
+      <c r="EX2" s="22"/>
+      <c r="EY2" s="22"/>
+      <c r="EZ2" s="20"/>
+      <c r="FA2" s="20"/>
+      <c r="FB2" s="20"/>
+      <c r="FC2" s="20"/>
     </row>
-    <row r="3" spans="1:159" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:159" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A3" s="7">
         <v>1</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" s="7">
         <v>172312001</v>
       </c>
       <c r="D3" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="E3" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="F3" s="15" t="s">
         <v>97</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>98</v>
       </c>
       <c r="G3" s="6"/>
       <c r="H3" s="3">
@@ -2279,24 +2279,24 @@
       </c>
       <c r="FC3" s="6"/>
     </row>
-    <row r="4" spans="1:159" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:159" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A4" s="7">
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="C4" s="7">
         <v>172312002</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="3">
@@ -2848,27 +2848,27 @@
         <v>Excellent</v>
       </c>
       <c r="FC4" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:159" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:159" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A5" s="7">
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" s="7">
         <v>172312003</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="3">
@@ -3420,27 +3420,27 @@
         <v>Excellent</v>
       </c>
       <c r="FC5" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:159" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:159" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A6" s="7">
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" s="7">
         <v>172312007</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G6" s="6"/>
       <c r="H6" s="3">
@@ -3992,27 +3992,27 @@
         <v>Excellent</v>
       </c>
       <c r="FC6" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:159" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:159" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A7" s="7">
         <v>5</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7" s="7">
         <v>172312008</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="3">
@@ -4564,27 +4564,27 @@
         <v>Excellent</v>
       </c>
       <c r="FC7" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:159" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:159" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A8" s="7">
         <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" s="7">
         <v>172312009</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="3">
@@ -5136,15 +5136,15 @@
         <v>Excellent</v>
       </c>
       <c r="FC8" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:159" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:159" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A9" s="7">
         <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C9" s="7">
         <v>172312010</v>
@@ -5152,7 +5152,7 @@
       <c r="D9" s="6"/>
       <c r="E9" s="15"/>
       <c r="F9" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="3">
@@ -5704,27 +5704,27 @@
         <v>Excellent</v>
       </c>
       <c r="FC9" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:159" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:159" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A10" s="7">
         <v>8</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C10" s="7">
         <v>172312011</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G10" s="6"/>
       <c r="H10" s="3">
@@ -6277,12 +6277,12 @@
       </c>
       <c r="FC10" s="6"/>
     </row>
-    <row r="11" spans="1:159" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:159" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A11" s="7">
         <v>9</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C11" s="7">
         <v>172312012</v>
@@ -6290,7 +6290,7 @@
       <c r="D11" s="6"/>
       <c r="E11" s="15"/>
       <c r="F11" s="15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G11" s="6"/>
       <c r="H11" s="3">
@@ -6843,24 +6843,24 @@
       </c>
       <c r="FC11" s="6"/>
     </row>
-    <row r="12" spans="1:159" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:159" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A12" s="7">
         <v>10</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12" s="7">
         <v>172312014</v>
       </c>
       <c r="D12" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E12" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="E12" s="15" t="s">
-        <v>75</v>
-      </c>
       <c r="F12" s="15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G12" s="6"/>
       <c r="H12" s="3">
@@ -7412,27 +7412,27 @@
         <v>Excellent</v>
       </c>
       <c r="FC12" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
-    <row r="13" spans="1:159" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:159" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A13" s="7">
         <v>11</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C13" s="7">
         <v>172312015</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G13" s="6"/>
       <c r="H13" s="3">
@@ -7985,12 +7985,12 @@
       </c>
       <c r="FC13" s="6"/>
     </row>
-    <row r="14" spans="1:159" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:159" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A14" s="7">
         <v>12</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C14" s="7">
         <v>172312016</v>
@@ -7998,7 +7998,7 @@
       <c r="D14" s="6"/>
       <c r="E14" s="15"/>
       <c r="F14" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G14" s="6"/>
       <c r="H14" s="3">
@@ -8551,24 +8551,24 @@
       </c>
       <c r="FC14" s="6"/>
     </row>
-    <row r="15" spans="1:159" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:159" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A15" s="7">
         <v>13</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C15" s="7">
         <v>172312017</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G15" s="6"/>
       <c r="H15" s="3">
@@ -9121,24 +9121,24 @@
       </c>
       <c r="FC15" s="6"/>
     </row>
-    <row r="16" spans="1:159" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:159" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A16" s="7">
         <v>14</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C16" s="7">
         <v>172312018</v>
       </c>
       <c r="D16" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E16" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="E16" s="15" t="s">
-        <v>77</v>
-      </c>
       <c r="F16" s="15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G16" s="6"/>
       <c r="H16" s="3">
@@ -9690,42 +9690,14 @@
         <v>Excellent</v>
       </c>
       <c r="FC16" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
-    <row r="17" spans="41:41" x14ac:dyDescent="0.2">
+    <row r="17" spans="41:41" x14ac:dyDescent="0.35">
       <c r="AO17" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="FB1:FB2"/>
-    <mergeCell ref="FC1:FC2"/>
-    <mergeCell ref="ET1:EU1"/>
-    <mergeCell ref="EV1:EW1"/>
-    <mergeCell ref="EX1:EX2"/>
-    <mergeCell ref="EY1:EY2"/>
-    <mergeCell ref="EZ1:EZ2"/>
-    <mergeCell ref="FA1:FA2"/>
-    <mergeCell ref="EM1:EQ1"/>
-    <mergeCell ref="DI1:DM1"/>
-    <mergeCell ref="ER1:ES1"/>
-    <mergeCell ref="DN1:DR1"/>
-    <mergeCell ref="DS1:DW1"/>
-    <mergeCell ref="DX1:EB1"/>
-    <mergeCell ref="EC1:EG1"/>
-    <mergeCell ref="EH1:EL1"/>
-    <mergeCell ref="DD1:DH1"/>
-    <mergeCell ref="BA1:BE1"/>
-    <mergeCell ref="BF1:BJ1"/>
-    <mergeCell ref="BK1:BO1"/>
-    <mergeCell ref="BP1:BT1"/>
-    <mergeCell ref="BU1:BY1"/>
-    <mergeCell ref="BZ1:CD1"/>
-    <mergeCell ref="CE1:CI1"/>
-    <mergeCell ref="CJ1:CN1"/>
-    <mergeCell ref="CO1:CS1"/>
-    <mergeCell ref="CT1:CX1"/>
-    <mergeCell ref="CY1:DC1"/>
     <mergeCell ref="AQ1:AU1"/>
     <mergeCell ref="AV1:AZ1"/>
     <mergeCell ref="A1:A2"/>
@@ -9742,6 +9714,34 @@
     <mergeCell ref="AG1:AK1"/>
     <mergeCell ref="AL1:AP1"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="DD1:DH1"/>
+    <mergeCell ref="BA1:BE1"/>
+    <mergeCell ref="BF1:BJ1"/>
+    <mergeCell ref="BK1:BO1"/>
+    <mergeCell ref="BP1:BT1"/>
+    <mergeCell ref="BU1:BY1"/>
+    <mergeCell ref="BZ1:CD1"/>
+    <mergeCell ref="CE1:CI1"/>
+    <mergeCell ref="CJ1:CN1"/>
+    <mergeCell ref="CO1:CS1"/>
+    <mergeCell ref="CT1:CX1"/>
+    <mergeCell ref="CY1:DC1"/>
+    <mergeCell ref="EM1:EQ1"/>
+    <mergeCell ref="DI1:DM1"/>
+    <mergeCell ref="ER1:ES1"/>
+    <mergeCell ref="DN1:DR1"/>
+    <mergeCell ref="DS1:DW1"/>
+    <mergeCell ref="DX1:EB1"/>
+    <mergeCell ref="EC1:EG1"/>
+    <mergeCell ref="EH1:EL1"/>
+    <mergeCell ref="FB1:FB2"/>
+    <mergeCell ref="FC1:FC2"/>
+    <mergeCell ref="ET1:EU1"/>
+    <mergeCell ref="EV1:EW1"/>
+    <mergeCell ref="EX1:EX2"/>
+    <mergeCell ref="EY1:EY2"/>
+    <mergeCell ref="EZ1:EZ2"/>
+    <mergeCell ref="FA1:FA2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>